<commit_message>
Feat: include HK/CH indices
</commit_message>
<xml_diff>
--- a/port_tickers.xlsx
+++ b/port_tickers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricky\Documents\Coding\aastock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BC7FC2-551C-43B8-821B-B4F85D8044EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6C7E7D-C245-4001-B54E-F3A7A4B13309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3705" yWindow="1140" windowWidth="10290" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Ident (BB_TCM)</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>BABA US Equity</t>
+  </si>
+  <si>
+    <t>HSCEI Index</t>
+  </si>
+  <si>
+    <t>SHSZ300 Index</t>
   </si>
 </sst>
 </file>
@@ -450,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,6 +532,16 @@
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD yahoo price source, indices & futures instruments
</commit_message>
<xml_diff>
--- a/port_tickers.xlsx
+++ b/port_tickers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricky\Documents\Coding\aastock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricky\Documents\Coding\tdp_prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6C7E7D-C245-4001-B54E-F3A7A4B13309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E35070-88E5-47BF-95DF-1A39F4DC49BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3705" yWindow="1140" windowWidth="10290" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Ident (BB_TCM)</t>
   </si>
@@ -44,24 +44,12 @@
     <t>1060 HK Equity</t>
   </si>
   <si>
-    <t>2823 HK Equity</t>
-  </si>
-  <si>
     <t>293 HK Equity</t>
   </si>
   <si>
-    <t>3033 HK Equity</t>
-  </si>
-  <si>
-    <t>700 HK Equity</t>
-  </si>
-  <si>
     <t>763 HK Equity</t>
   </si>
   <si>
-    <t>857 HK Equity</t>
-  </si>
-  <si>
     <t>KWEB US Equity</t>
   </si>
   <si>
@@ -81,6 +69,24 @@
   </si>
   <si>
     <t>SHSZ300 Index</t>
+  </si>
+  <si>
+    <t>11 HK Equity</t>
+  </si>
+  <si>
+    <t>5 HK Equity</t>
+  </si>
+  <si>
+    <t>XIN9I Index</t>
+  </si>
+  <si>
+    <t>NDX Index</t>
+  </si>
+  <si>
+    <t>XUU1 Index</t>
+  </si>
+  <si>
+    <t>HCTV1 Index</t>
   </si>
 </sst>
 </file>
@@ -456,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +477,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -486,61 +492,71 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add more futures on yahoo(ES,NQ,XU) and AA(front and next month)
</commit_message>
<xml_diff>
--- a/port_tickers.xlsx
+++ b/port_tickers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricky\Documents\Coding\tdp_prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E35070-88E5-47BF-95DF-1A39F4DC49BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF84A371-6248-4234-8771-D324E9AC8B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3705" yWindow="1140" windowWidth="10290" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Ident (BB_TCM)</t>
   </si>
@@ -44,9 +44,6 @@
     <t>1060 HK Equity</t>
   </si>
   <si>
-    <t>293 HK Equity</t>
-  </si>
-  <si>
     <t>763 HK Equity</t>
   </si>
   <si>
@@ -87,6 +84,15 @@
   </si>
   <si>
     <t>HCTV1 Index</t>
+  </si>
+  <si>
+    <t>XUV1 Index</t>
+  </si>
+  <si>
+    <t>ESZ1 Index</t>
+  </si>
+  <si>
+    <t>HIU1 Index</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,7 +483,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -487,7 +493,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -497,67 +503,87 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -569,7 +595,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>